<commit_message>
adding astra db fetching
</commit_message>
<xml_diff>
--- a/user_info.xlsx
+++ b/user_info.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -615,6 +615,70 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>subhan</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>0987654321</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>sd@sk.com</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>pk</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2025-08-11 21:02:45</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>session_1754928140</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>subhan</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>0987654432</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>sad@sk.com</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>wef</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2025-08-11 21:11:53</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>session_1754928656</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added astra + tmdb support
</commit_message>
<xml_diff>
--- a/user_info.xlsx
+++ b/user_info.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -899,6 +899,50 @@
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>daf</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>fds</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>dsf</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>dsf</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>ds</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>